<commit_message>
lastest commit for all May2020 files
</commit_message>
<xml_diff>
--- a/Code/Output/April_2020/reason_codes.xlsx
+++ b/Code/Output/April_2020/reason_codes.xlsx
@@ -1,55 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\Output\April_2020\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81B0F58-E244-4DB4-B08A-FE9B1D40BE8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="24870" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">Reason_Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORDER ENTRY ERROR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELECTRICAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORDER PROCESSING ERROR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHANGES - NOT NEEDED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHIPPING ERROR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FREIGHT CARRIER ERROR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHANGES -  REORDERED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PICKING ERROR</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Reason_Code</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>ORDER ENTRY ERROR</t>
+  </si>
+  <si>
+    <t>ELECTRICAL</t>
+  </si>
+  <si>
+    <t>ORDER PROCESSING ERROR</t>
+  </si>
+  <si>
+    <t>CHANGES - NOT NEEDED</t>
+  </si>
+  <si>
+    <t>SHIPPING ERROR</t>
+  </si>
+  <si>
+    <t>FREIGHT CARRIER ERROR</t>
+  </si>
+  <si>
+    <t>CHANGES -  REORDERED</t>
+  </si>
+  <si>
+    <t>PICKING ERROR</t>
+  </si>
+  <si>
+    <t># of RMAs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -85,6 +105,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -366,87 +395,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>735</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
+        <v>65</v>
+      </c>
+      <c r="C3">
         <v>348</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
         <v>80</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
         <v>58</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
         <v>44</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
         <v>25</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>